<commit_message>
source data - created new sheet for multiple WT:DI treatments -> saved to csv file call 'yield_comparisons'
</commit_message>
<xml_diff>
--- a/Source_Data/Source_Data_3.xlsx
+++ b/Source_Data/Source_Data_3.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jharris387/Dropbox (Personal)/Cycling_ms/Source_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jharris387/Dropbox (Personal)/Cycling_ms_share/Source_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D44A9C-FE74-FA44-97B3-63C2AD1989A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8DA8A0-A09D-3646-83AA-20C672B1C2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="2400" windowWidth="25640" windowHeight="13180" xr2:uid="{91DC55ED-DCBF-0742-BECB-7685D0DD4FEB}"/>
+    <workbookView xWindow="1820" yWindow="2400" windowWidth="25640" windowHeight="13180" activeTab="1" xr2:uid="{91DC55ED-DCBF-0742-BECB-7685D0DD4FEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Figures 3A,4A" sheetId="3" r:id="rId1"/>
-    <sheet name="Figure 3B" sheetId="7" r:id="rId2"/>
-    <sheet name="Figure 3C - DI-enriched stock" sheetId="5" r:id="rId3"/>
-    <sheet name="WT stock" sheetId="4" r:id="rId4"/>
+    <sheet name="yield comparisons" sheetId="8" r:id="rId2"/>
+    <sheet name="Figure 3B" sheetId="7" r:id="rId3"/>
+    <sheet name="Figure 3C - DI-enriched stock" sheetId="5" r:id="rId4"/>
+    <sheet name="WT stock" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>Experiment (USING MA primers; intended ratios met)</t>
   </si>
@@ -273,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -554,12 +555,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -590,7 +606,6 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -643,7 +658,7 @@
     <xf numFmtId="11" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -651,7 +666,6 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -682,18 +696,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1016,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CD68D8-95BD-5B41-ABEA-51C5DEF98001}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1028,76 +1047,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="73" t="s">
+      <c r="C1" s="69"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="74"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="73" t="s">
+      <c r="F1" s="72"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="74"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="73" t="s">
+      <c r="I1" s="72"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="74"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="73" t="s">
+      <c r="L1" s="72"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="74"/>
-      <c r="P1" s="75"/>
-      <c r="R1" s="66" t="s">
+      <c r="O1" s="72"/>
+      <c r="P1" s="73"/>
+      <c r="R1" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="64">
+      <c r="S1" s="63">
         <f>1-PRODUCT('WT stock'!D4:D11)</f>
         <v>0.25698656540832132</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="67">
+      <c r="B2" s="65">
         <v>1886666.66666667</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="67">
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="65">
         <v>5800000</v>
       </c>
-      <c r="F2" s="68"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="67">
+      <c r="F2" s="66"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="65">
         <v>6440000</v>
       </c>
-      <c r="I2" s="68"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="67">
+      <c r="I2" s="66"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="65">
         <v>30533333.333333299</v>
       </c>
-      <c r="L2" s="68"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="67">
+      <c r="L2" s="66"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="65">
         <v>156333333.33333299</v>
       </c>
-      <c r="O2" s="68"/>
-      <c r="P2" s="69"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="64"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="67"/>
+      <c r="R2" s="64"/>
+      <c r="S2" s="63"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1">
@@ -1160,16 +1179,16 @@
         <f>1/101</f>
         <v>9.9009900990099011E-3</v>
       </c>
-      <c r="R3" s="66" t="s">
+      <c r="R3" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="65">
+      <c r="S3" s="63">
         <f>1-PRODUCT('Figure 3C - DI-enriched stock'!D4:D11)</f>
         <v>0.9999829810259584</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1">
@@ -1232,61 +1251,61 @@
         <f t="shared" si="0"/>
         <v>0.99009900990099009</v>
       </c>
-      <c r="R4" s="66"/>
-      <c r="S4" s="65"/>
+      <c r="R4" s="64"/>
+      <c r="S4" s="63"/>
     </row>
     <row r="5" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="26">
         <v>55853</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="27">
         <v>37238.443440000061</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="28">
         <v>432946.58524646168</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="26">
         <v>3916950.7554835393</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="27">
         <v>3981022.6197704319</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="28">
         <v>3968452.3403683202</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="26">
         <v>3441665.3860191684</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I5" s="27">
         <v>3502987.5133261173</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="28">
         <v>3445055.7823743955</v>
       </c>
-      <c r="K5" s="27">
+      <c r="K5" s="26">
         <v>227000</v>
       </c>
-      <c r="L5" s="28">
+      <c r="L5" s="27">
         <v>522365.13354309648</v>
       </c>
-      <c r="M5" s="29">
+      <c r="M5" s="28">
         <v>522365.13354309648</v>
       </c>
-      <c r="N5" s="27">
+      <c r="N5" s="26">
         <v>24200000.000000015</v>
       </c>
-      <c r="O5" s="28">
+      <c r="O5" s="27">
         <v>50660955.496401787</v>
       </c>
-      <c r="P5" s="29">
+      <c r="P5" s="28">
         <v>32273653.123116717</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="5">
@@ -1351,7 +1370,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="5">
@@ -1416,7 +1435,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5">
@@ -1481,7 +1500,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="5">
@@ -1546,7 +1565,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="23" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="5">
@@ -1611,72 +1630,72 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="61">
+      <c r="B11" s="60">
         <f>B9/2000000</f>
         <v>0.68015957528369364</v>
       </c>
-      <c r="C11" s="62">
+      <c r="C11" s="61">
         <f t="shared" ref="C11:P12" si="5">C9/2000000</f>
         <v>0.68707500808521693</v>
       </c>
-      <c r="D11" s="63">
+      <c r="D11" s="62">
         <f t="shared" si="5"/>
         <v>0.54006677531546188</v>
       </c>
-      <c r="E11" s="61">
+      <c r="E11" s="60">
         <f t="shared" si="5"/>
         <v>0.63597004155911929</v>
       </c>
-      <c r="F11" s="62">
+      <c r="F11" s="61">
         <f t="shared" si="5"/>
         <v>0.614330784746285</v>
       </c>
-      <c r="G11" s="63">
+      <c r="G11" s="62">
         <f t="shared" si="5"/>
         <v>0.61857619741249681</v>
       </c>
-      <c r="H11" s="61">
+      <c r="H11" s="60">
         <f t="shared" si="5"/>
         <v>0.55696348204199408</v>
       </c>
-      <c r="I11" s="62">
+      <c r="I11" s="61">
         <f t="shared" si="5"/>
         <v>0.5455724300253697</v>
       </c>
-      <c r="J11" s="63">
+      <c r="J11" s="62">
         <f t="shared" si="5"/>
         <v>0.55633369010659595</v>
       </c>
-      <c r="K11" s="61">
+      <c r="K11" s="60">
         <f t="shared" si="5"/>
         <v>1.023780483949237</v>
       </c>
-      <c r="L11" s="62">
+      <c r="L11" s="61">
         <f t="shared" si="5"/>
         <v>1.0138027325652419</v>
       </c>
-      <c r="M11" s="63">
+      <c r="M11" s="62">
         <f t="shared" si="5"/>
         <v>1.0138027325652419</v>
       </c>
-      <c r="N11" s="61">
+      <c r="N11" s="60">
         <f t="shared" si="5"/>
         <v>0.48713722376757401</v>
       </c>
-      <c r="O11" s="62">
+      <c r="O11" s="61">
         <f t="shared" si="5"/>
         <v>0.38958336605752464</v>
       </c>
-      <c r="P11" s="63">
+      <c r="P11" s="62">
         <f t="shared" si="5"/>
         <v>0.45737200957944973</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="8">
@@ -1741,125 +1760,124 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="20"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="19"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="54">
+      <c r="B14" s="53">
         <v>9879330.0557718147</v>
       </c>
-      <c r="C14" s="55">
+      <c r="C14" s="54">
         <v>5555555.5555555616</v>
       </c>
-      <c r="D14" s="56">
+      <c r="D14" s="55">
         <v>9879330.0557718147</v>
       </c>
-      <c r="E14" s="54">
+      <c r="E14" s="53">
         <v>17600000</v>
       </c>
-      <c r="F14" s="55">
+      <c r="F14" s="54">
         <v>5560000</v>
       </c>
-      <c r="G14" s="56">
+      <c r="G14" s="55">
         <v>9880000</v>
       </c>
-      <c r="H14" s="54">
+      <c r="H14" s="53">
         <v>1760000</v>
       </c>
-      <c r="I14" s="55">
+      <c r="I14" s="54">
         <v>5560000</v>
       </c>
-      <c r="J14" s="56">
+      <c r="J14" s="55">
         <v>3120000</v>
       </c>
-      <c r="K14" s="54">
+      <c r="K14" s="53">
         <v>988000</v>
       </c>
-      <c r="L14" s="55">
+      <c r="L14" s="54">
         <v>312000</v>
       </c>
-      <c r="M14" s="56">
+      <c r="M14" s="55">
         <v>312000</v>
       </c>
-      <c r="N14" s="54">
+      <c r="N14" s="53">
         <v>312000</v>
       </c>
-      <c r="O14" s="55">
+      <c r="O14" s="54">
         <v>176000</v>
       </c>
-      <c r="P14" s="56">
+      <c r="P14" s="55">
         <v>556000</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="58">
+      <c r="B15" s="57">
         <v>30000000</v>
       </c>
-      <c r="C15" s="59">
+      <c r="C15" s="58">
         <v>196000000</v>
       </c>
-      <c r="D15" s="60">
+      <c r="D15" s="59">
         <v>219000000</v>
       </c>
-      <c r="E15" s="58">
+      <c r="E15" s="57">
         <v>228000000</v>
       </c>
-      <c r="F15" s="59">
+      <c r="F15" s="58">
         <v>221000000</v>
       </c>
-      <c r="G15" s="60" t="s">
+      <c r="G15" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="58">
+      <c r="H15" s="57">
         <v>334000000</v>
       </c>
-      <c r="I15" s="59">
+      <c r="I15" s="58">
         <v>135000000</v>
       </c>
-      <c r="J15" s="60">
+      <c r="J15" s="59">
         <v>279000000</v>
       </c>
-      <c r="K15" s="58">
+      <c r="K15" s="57">
         <v>372000000</v>
       </c>
-      <c r="L15" s="59">
+      <c r="L15" s="58">
         <v>355000000</v>
       </c>
-      <c r="M15" s="60">
+      <c r="M15" s="59">
         <v>312000000</v>
       </c>
-      <c r="N15" s="58">
+      <c r="N15" s="57">
         <v>161000000</v>
       </c>
-      <c r="O15" s="59">
+      <c r="O15" s="58">
         <v>685000000</v>
       </c>
-      <c r="P15" s="60">
+      <c r="P15" s="59">
         <v>275000000</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="13">
@@ -1944,6 +1962,118 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40C143D-1D97-F14A-819E-DB2A96540498}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="80"/>
+      <c r="B1" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="80" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="81">
+        <f>'Figures 3A,4A'!B15</f>
+        <v>30000000</v>
+      </c>
+      <c r="C2" s="81">
+        <f>'Figures 3A,4A'!C15</f>
+        <v>196000000</v>
+      </c>
+      <c r="D2" s="81">
+        <f>'Figures 3A,4A'!D15</f>
+        <v>219000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="81">
+        <f>'Figures 3A,4A'!E15</f>
+        <v>228000000</v>
+      </c>
+      <c r="C3" s="81">
+        <f>'Figures 3A,4A'!F15</f>
+        <v>221000000</v>
+      </c>
+      <c r="D3" s="81" t="str">
+        <f>'Figures 3A,4A'!G15</f>
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="79" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="81">
+        <f>'Figures 3A,4A'!H15</f>
+        <v>334000000</v>
+      </c>
+      <c r="C4" s="81">
+        <f>'Figures 3A,4A'!I15</f>
+        <v>135000000</v>
+      </c>
+      <c r="D4" s="81">
+        <f>'Figures 3A,4A'!J15</f>
+        <v>279000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="81">
+        <f>'Figures 3A,4A'!K15</f>
+        <v>372000000</v>
+      </c>
+      <c r="C5" s="81">
+        <f>'Figures 3A,4A'!L15</f>
+        <v>355000000</v>
+      </c>
+      <c r="D5" s="81">
+        <f>'Figures 3A,4A'!M15</f>
+        <v>312000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="82">
+        <f>'Figures 3A,4A'!N15</f>
+        <v>161000000</v>
+      </c>
+      <c r="C6" s="82">
+        <f>'Figures 3A,4A'!O15</f>
+        <v>685000000</v>
+      </c>
+      <c r="D6" s="82">
+        <f>'Figures 3A,4A'!P15</f>
+        <v>275000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08DE016-E735-744E-8E0A-39442A04CDB7}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1957,50 +2087,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="78"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="76"/>
     </row>
     <row r="2" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="46" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="51">
+      <c r="B3" s="50">
         <v>14300000</v>
       </c>
-      <c r="C3" s="52">
+      <c r="C3" s="51">
         <v>11800000</v>
       </c>
-      <c r="D3" s="53">
+      <c r="D3" s="52">
         <v>13700000</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="7">
         <v>5290928</v>
       </c>
-      <c r="C4" s="48">
+      <c r="C4" s="47">
         <v>5508908</v>
       </c>
-      <c r="D4" s="49">
+      <c r="D4" s="48">
         <v>4603664</v>
       </c>
     </row>
@@ -2012,7 +2142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D531B7C-66C5-E34A-B0B5-AB901F499CC2}">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -2029,155 +2159,155 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
     </row>
     <row r="2" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="37" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="20">
         <v>2760209150.6620922</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="20">
         <v>184310205.82631055</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="41">
         <f>C4/B4</f>
         <v>6.6774E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <v>2759320909.5838418</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="23">
         <v>217710419.76616511</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="42">
         <f t="shared" ref="D5:D11" si="0">C5/B5</f>
         <v>7.8899999999999998E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>2756878246.6186543</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="23">
         <v>180978029.37752816</v>
       </c>
-      <c r="D6" s="43">
+      <c r="D6" s="42">
         <f t="shared" si="0"/>
         <v>6.5645999999999996E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="23">
         <v>2755767945.2708416</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="23">
         <v>757224404.46563137</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="42">
         <f t="shared" si="0"/>
         <v>0.27477800000000002</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="23">
         <v>2761319452.0099044</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="23">
         <v>2142880540.9405062</v>
       </c>
-      <c r="D8" s="43">
+      <c r="D8" s="42">
         <f t="shared" si="0"/>
         <v>0.77603500000000003</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="23">
         <v>2756878246.6186543</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="23">
         <v>636202036.09394026</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="42">
         <f t="shared" si="0"/>
         <v>0.230769</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="23">
         <v>2753547342.5752163</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="23">
         <v>2753547192.5665417</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="42">
         <f t="shared" si="0"/>
         <v>0.99999994552166493</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="21">
         <v>2764650356.0533423</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="21">
         <v>2764650356.0540338</v>
       </c>
-      <c r="D11" s="44">
+      <c r="D11" s="43">
         <f t="shared" si="0"/>
         <v>1.00000000000025</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="36"/>
-      <c r="B14" s="37"/>
-    </row>
-    <row r="15" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="36"/>
-      <c r="B15" s="37"/>
+    <row r="14" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="35"/>
+      <c r="B14" s="36"/>
+    </row>
+    <row r="15" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="35"/>
+      <c r="B15" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2187,7 +2317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C08E6AD0-69FC-664A-B5BF-20848FF1953D}">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -2204,155 +2334,155 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
     </row>
     <row r="2" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="37" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="40">
+      <c r="B4" s="39">
         <v>2031976215.43261</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="40">
         <v>1661681061.7894638</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="41">
         <f>C4/B4</f>
         <v>0.81776599999999999</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="31">
         <v>2031793952.43665</v>
       </c>
       <c r="C5" s="12">
         <v>2031793941.3927629</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="42">
         <f t="shared" ref="D5:D11" si="0">C5/B5</f>
         <v>0.99999999456446498</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="31">
         <v>2029798737.4220333</v>
       </c>
       <c r="C6" s="12">
         <v>1844264983.8279724</v>
       </c>
-      <c r="D6" s="43">
+      <c r="D6" s="42">
         <f t="shared" si="0"/>
         <v>0.90859500000000004</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="31">
         <v>2028468594.1515601</v>
       </c>
       <c r="C7" s="12">
         <v>2028467712.1027253</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="42">
         <f t="shared" si="0"/>
         <v>0.99999956516515098</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="31">
         <v>2029873977.1561501</v>
       </c>
       <c r="C8" s="12">
         <v>2029873977.1562312</v>
       </c>
-      <c r="D8" s="43">
+      <c r="D8" s="42">
         <f t="shared" si="0"/>
         <v>1.00000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="31">
         <v>2028444526.0841501</v>
       </c>
       <c r="C9" s="12">
         <v>2028444526.081213</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="42">
         <f t="shared" si="0"/>
         <v>0.99999999999855205</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="31">
         <v>2021817877.3797448</v>
       </c>
       <c r="C10" s="12">
         <v>2021816899.7674253</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="42">
         <f t="shared" si="0"/>
         <v>0.99999951646865404</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="34">
+      <c r="B11" s="33">
         <v>2031793952.4326053</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="34">
         <v>2031783075.1353204</v>
       </c>
-      <c r="D11" s="44">
+      <c r="D11" s="43">
         <f t="shared" si="0"/>
         <v>0.99999464645651115</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="36"/>
-      <c r="B14" s="37"/>
-    </row>
-    <row r="15" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="36"/>
-      <c r="B15" s="37"/>
+    <row r="14" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="35"/>
+      <c r="B14" s="36"/>
+    </row>
+    <row r="15" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="35"/>
+      <c r="B15" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>